<commit_message>
update extension treatment 9356d7d0fb5f9145a7c85a328feccc8f45b4f950
</commit_message>
<xml_diff>
--- a/update-mapping-pn13/ig/StructureDefinition-oncofair-careplan.xlsx
+++ b/update-mapping-pn13/ig/StructureDefinition-oncofair-careplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2220" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2220" uniqueCount="419">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-23T14:57:19+00:00</t>
+    <t>2024-05-27T07:09:09+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -474,7 +474,7 @@
 </t>
   </si>
   <si>
-    <t>Extension créée dans le cadre d'OncoFAIR</t>
+    <t>Extension created as part of OncoFAIR,Extension créée dans le cadre d'OncoFAIR</t>
   </si>
   <si>
     <t>CarePlan.extension:oncofair-pharmacist-advice</t>
@@ -485,6 +485,9 @@
   <si>
     <t xml:space="preserve">Extension {http://ltsi.univ-rennes.fr/StructureDefinition/oncofair-pharmacist-advice}
 </t>
+  </si>
+  <si>
+    <t>Extension créée dans le cadre d'OncoFAIR</t>
   </si>
   <si>
     <t>CarePlan.modifierExtension</t>
@@ -2893,7 +2896,7 @@
         <v>137</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -2976,14 +2979,14 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" t="s" s="2">
@@ -3005,16 +3008,16 @@
         <v>136</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="N12" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="O12" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="P12" t="s" s="2">
         <v>79</v>
@@ -3063,7 +3066,7 @@
         <v>79</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>77</v>
@@ -3095,10 +3098,10 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
@@ -3121,19 +3124,19 @@
         <v>90</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="N13" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="O13" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="P13" t="s" s="2">
         <v>79</v>
@@ -3182,7 +3185,7 @@
         <v>79</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>77</v>
@@ -3197,27 +3200,27 @@
         <v>101</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="AN13" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AO13" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -3240,13 +3243,13 @@
         <v>90</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -3297,7 +3300,7 @@
         <v>79</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>77</v>
@@ -3315,13 +3318,13 @@
         <v>79</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AM14" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AN14" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AO14" t="s" s="2">
         <v>79</v>
@@ -3329,10 +3332,10 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
@@ -3358,13 +3361,13 @@
         <v>103</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="O15" s="2"/>
       <c r="P15" t="s" s="2">
@@ -3414,7 +3417,7 @@
         <v>79</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>77</v>
@@ -3432,13 +3435,13 @@
         <v>79</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="AM15" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>79</v>
@@ -3446,14 +3449,14 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" t="s" s="2">
@@ -3472,17 +3475,17 @@
         <v>90</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="P16" t="s" s="2">
         <v>79</v>
@@ -3531,7 +3534,7 @@
         <v>79</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>77</v>
@@ -3546,10 +3549,10 @@
         <v>101</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AM16" t="s" s="2">
         <v>79</v>
@@ -3563,14 +3566,14 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" t="s" s="2">
@@ -3589,19 +3592,19 @@
         <v>90</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O17" t="s" s="2">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="P17" t="s" s="2">
         <v>79</v>
@@ -3650,7 +3653,7 @@
         <v>79</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>77</v>
@@ -3668,7 +3671,7 @@
         <v>79</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AM17" t="s" s="2">
         <v>79</v>
@@ -3682,10 +3685,10 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3708,16 +3711,16 @@
         <v>90</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" t="s" s="2">
@@ -3767,7 +3770,7 @@
         <v>79</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>77</v>
@@ -3799,10 +3802,10 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3828,16 +3831,16 @@
         <v>109</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="O19" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="P19" t="s" s="2">
         <v>79</v>
@@ -3865,10 +3868,10 @@
         <v>113</v>
       </c>
       <c r="Y19" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="Z19" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="AA19" t="s" s="2">
         <v>79</v>
@@ -3886,7 +3889,7 @@
         <v>79</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>89</v>
@@ -3901,27 +3904,27 @@
         <v>101</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AO19" t="s" s="2">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3947,16 +3950,16 @@
         <v>109</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="O20" t="s" s="2">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="P20" t="s" s="2">
         <v>79</v>
@@ -3984,10 +3987,10 @@
         <v>113</v>
       </c>
       <c r="Y20" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="Z20" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AA20" t="s" s="2">
         <v>79</v>
@@ -4005,7 +4008,7 @@
         <v>79</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>89</v>
@@ -4023,7 +4026,7 @@
         <v>79</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AM20" t="s" s="2">
         <v>79</v>
@@ -4037,10 +4040,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -4063,19 +4066,19 @@
         <v>90</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="O21" t="s" s="2">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="P21" t="s" s="2">
         <v>79</v>
@@ -4100,13 +4103,13 @@
         <v>79</v>
       </c>
       <c r="X21" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="Y21" t="s" s="2">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="Z21" t="s" s="2">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AA21" t="s" s="2">
         <v>79</v>
@@ -4124,7 +4127,7 @@
         <v>79</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>77</v>
@@ -4145,7 +4148,7 @@
         <v>79</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AN21" t="s" s="2">
         <v>79</v>
@@ -4156,10 +4159,10 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4182,13 +4185,13 @@
         <v>90</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -4239,7 +4242,7 @@
         <v>79</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>77</v>
@@ -4254,7 +4257,7 @@
         <v>101</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AL22" t="s" s="2">
         <v>79</v>
@@ -4271,10 +4274,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4297,17 +4300,17 @@
         <v>90</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="P23" t="s" s="2">
         <v>79</v>
@@ -4356,7 +4359,7 @@
         <v>79</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>77</v>
@@ -4377,7 +4380,7 @@
         <v>79</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="AN23" t="s" s="2">
         <v>79</v>
@@ -4388,14 +4391,14 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s" s="2">
@@ -4414,13 +4417,13 @@
         <v>90</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -4471,7 +4474,7 @@
         <v>79</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>89</v>
@@ -4489,24 +4492,24 @@
         <v>79</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AO24" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4529,16 +4532,16 @@
         <v>90</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" t="s" s="2">
@@ -4588,7 +4591,7 @@
         <v>79</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>77</v>
@@ -4606,28 +4609,28 @@
         <v>79</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" t="s" s="2">
@@ -4646,19 +4649,19 @@
         <v>90</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="O26" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>79</v>
@@ -4707,7 +4710,7 @@
         <v>79</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>77</v>
@@ -4725,28 +4728,28 @@
         <v>79</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="AO26" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" t="s" s="2">
@@ -4765,13 +4768,13 @@
         <v>90</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
@@ -4822,7 +4825,7 @@
         <v>79</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>77</v>
@@ -4840,13 +4843,13 @@
         <v>79</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AO27" t="s" s="2">
         <v>79</v>
@@ -4854,10 +4857,10 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4880,16 +4883,16 @@
         <v>90</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
@@ -4939,7 +4942,7 @@
         <v>79</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>77</v>
@@ -4957,10 +4960,10 @@
         <v>79</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>79</v>
@@ -4971,10 +4974,10 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4997,16 +5000,16 @@
         <v>79</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" t="s" s="2">
@@ -5056,7 +5059,7 @@
         <v>79</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>77</v>
@@ -5088,10 +5091,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5114,17 +5117,17 @@
         <v>79</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="P30" t="s" s="2">
         <v>79</v>
@@ -5173,7 +5176,7 @@
         <v>79</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>77</v>
@@ -5191,10 +5194,10 @@
         <v>79</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>79</v>
@@ -5205,10 +5208,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5231,19 +5234,19 @@
         <v>90</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="O31" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>79</v>
@@ -5268,13 +5271,13 @@
         <v>79</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="Z31" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AA31" t="s" s="2">
         <v>79</v>
@@ -5292,7 +5295,7 @@
         <v>79</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>77</v>
@@ -5310,24 +5313,24 @@
         <v>79</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5350,19 +5353,19 @@
         <v>79</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="O32" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="P32" t="s" s="2">
         <v>79</v>
@@ -5411,7 +5414,7 @@
         <v>79</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>77</v>
@@ -5429,7 +5432,7 @@
         <v>79</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>79</v>
@@ -5443,10 +5446,10 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5469,19 +5472,19 @@
         <v>79</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="O33" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="P33" t="s" s="2">
         <v>79</v>
@@ -5530,7 +5533,7 @@
         <v>79</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>77</v>
@@ -5554,18 +5557,18 @@
         <v>79</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AO33" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5588,17 +5591,17 @@
         <v>79</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="P34" t="s" s="2">
         <v>79</v>
@@ -5647,7 +5650,7 @@
         <v>79</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>77</v>
@@ -5665,13 +5668,13 @@
         <v>79</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AO34" t="s" s="2">
         <v>79</v>
@@ -5679,10 +5682,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5705,13 +5708,13 @@
         <v>79</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -5762,7 +5765,7 @@
         <v>79</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>77</v>
@@ -5771,7 +5774,7 @@
         <v>89</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>79</v>
@@ -5786,7 +5789,7 @@
         <v>79</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AO35" t="s" s="2">
         <v>79</v>
@@ -5794,14 +5797,14 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s" s="2">
@@ -5823,13 +5826,13 @@
         <v>136</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="O36" s="2"/>
       <c r="P36" t="s" s="2">
@@ -5879,7 +5882,7 @@
         <v>79</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>77</v>
@@ -5903,7 +5906,7 @@
         <v>79</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AO36" t="s" s="2">
         <v>79</v>
@@ -5911,14 +5914,14 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" t="s" s="2">
@@ -5940,16 +5943,16 @@
         <v>136</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="O37" t="s" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="P37" t="s" s="2">
         <v>79</v>
@@ -5998,7 +6001,7 @@
         <v>79</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>77</v>
@@ -6030,10 +6033,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6056,19 +6059,19 @@
         <v>79</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="O38" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>79</v>
@@ -6093,13 +6096,13 @@
         <v>79</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="Z38" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="AA38" t="s" s="2">
         <v>79</v>
@@ -6117,7 +6120,7 @@
         <v>79</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>77</v>
@@ -6135,13 +6138,13 @@
         <v>79</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AO38" t="s" s="2">
         <v>79</v>
@@ -6149,10 +6152,10 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6175,19 +6178,19 @@
         <v>79</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="O39" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="P39" t="s" s="2">
         <v>79</v>
@@ -6236,7 +6239,7 @@
         <v>79</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>77</v>
@@ -6260,18 +6263,18 @@
         <v>79</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AO39" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6294,19 +6297,19 @@
         <v>79</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="O40" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="P40" t="s" s="2">
         <v>79</v>
@@ -6355,7 +6358,7 @@
         <v>79</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>77</v>
@@ -6373,13 +6376,13 @@
         <v>79</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AN40" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AO40" t="s" s="2">
         <v>79</v>
@@ -6387,10 +6390,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6413,17 +6416,17 @@
         <v>79</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="P41" t="s" s="2">
         <v>79</v>
@@ -6460,7 +6463,7 @@
         <v>79</v>
       </c>
       <c r="AB41" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AC41" s="2"/>
       <c r="AD41" t="s" s="2">
@@ -6470,7 +6473,7 @@
         <v>140</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>77</v>
@@ -6488,27 +6491,27 @@
         <v>79</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AO41" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C42" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="D42" t="s" s="2">
         <v>79</v>
@@ -6530,17 +6533,17 @@
         <v>79</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="P42" t="s" s="2">
         <v>79</v>
@@ -6589,7 +6592,7 @@
         <v>79</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>77</v>
@@ -6604,27 +6607,27 @@
         <v>101</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM42" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AO42" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6650,10 +6653,10 @@
         <v>91</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -6665,7 +6668,7 @@
         <v>79</v>
       </c>
       <c r="S43" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="T43" t="s" s="2">
         <v>79</v>
@@ -6704,7 +6707,7 @@
         <v>79</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>77</v>
@@ -6713,7 +6716,7 @@
         <v>89</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>79</v>
@@ -6728,7 +6731,7 @@
         <v>79</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AO43" t="s" s="2">
         <v>79</v>
@@ -6736,14 +6739,14 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" t="s" s="2">
@@ -6765,13 +6768,13 @@
         <v>136</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="O44" s="2"/>
       <c r="P44" t="s" s="2">
@@ -6812,7 +6815,7 @@
         <v>139</v>
       </c>
       <c r="AC44" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AD44" t="s" s="2">
         <v>79</v>
@@ -6821,7 +6824,7 @@
         <v>140</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>77</v>
@@ -6845,7 +6848,7 @@
         <v>79</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AO44" t="s" s="2">
         <v>79</v>
@@ -6853,10 +6856,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6879,16 +6882,16 @@
         <v>90</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
@@ -6938,7 +6941,7 @@
         <v>79</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>77</v>
@@ -6962,7 +6965,7 @@
         <v>79</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>134</v>
@@ -6970,10 +6973,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -6996,13 +6999,13 @@
         <v>90</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -7053,7 +7056,7 @@
         <v>79</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>77</v>
@@ -7077,7 +7080,7 @@
         <v>79</v>
       </c>
       <c r="AN46" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AO46" t="s" s="2">
         <v>134</v>
@@ -7085,10 +7088,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7111,13 +7114,13 @@
         <v>90</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -7168,7 +7171,7 @@
         <v>79</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>89</v>
@@ -7192,7 +7195,7 @@
         <v>79</v>
       </c>
       <c r="AN47" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AO47" t="s" s="2">
         <v>134</v>
@@ -7200,13 +7203,13 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C48" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D48" t="s" s="2">
         <v>79</v>
@@ -7228,17 +7231,17 @@
         <v>79</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="P48" t="s" s="2">
         <v>79</v>
@@ -7287,7 +7290,7 @@
         <v>79</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>77</v>
@@ -7302,27 +7305,27 @@
         <v>101</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM48" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AO48" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7348,10 +7351,10 @@
         <v>91</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -7363,7 +7366,7 @@
         <v>79</v>
       </c>
       <c r="S49" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="T49" t="s" s="2">
         <v>79</v>
@@ -7402,7 +7405,7 @@
         <v>79</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>77</v>
@@ -7411,7 +7414,7 @@
         <v>89</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>79</v>
@@ -7426,7 +7429,7 @@
         <v>79</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AO49" t="s" s="2">
         <v>79</v>
@@ -7434,14 +7437,14 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s" s="2">
@@ -7463,13 +7466,13 @@
         <v>136</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="O50" s="2"/>
       <c r="P50" t="s" s="2">
@@ -7510,7 +7513,7 @@
         <v>139</v>
       </c>
       <c r="AC50" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AD50" t="s" s="2">
         <v>79</v>
@@ -7519,7 +7522,7 @@
         <v>140</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>77</v>
@@ -7543,7 +7546,7 @@
         <v>79</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AO50" t="s" s="2">
         <v>79</v>
@@ -7551,10 +7554,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7577,16 +7580,16 @@
         <v>90</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="O51" s="2"/>
       <c r="P51" t="s" s="2">
@@ -7636,7 +7639,7 @@
         <v>79</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>77</v>
@@ -7660,7 +7663,7 @@
         <v>79</v>
       </c>
       <c r="AN51" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AO51" t="s" s="2">
         <v>134</v>
@@ -7668,10 +7671,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7694,13 +7697,13 @@
         <v>90</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -7751,7 +7754,7 @@
         <v>79</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>77</v>
@@ -7775,7 +7778,7 @@
         <v>79</v>
       </c>
       <c r="AN52" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AO52" t="s" s="2">
         <v>134</v>
@@ -7783,10 +7786,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7809,13 +7812,13 @@
         <v>90</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -7866,7 +7869,7 @@
         <v>79</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>89</v>
@@ -7890,7 +7893,7 @@
         <v>79</v>
       </c>
       <c r="AN53" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AO53" t="s" s="2">
         <v>134</v>
@@ -7898,13 +7901,13 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C54" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D54" t="s" s="2">
         <v>79</v>
@@ -7926,17 +7929,17 @@
         <v>79</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="N54" s="2"/>
       <c r="O54" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="P54" t="s" s="2">
         <v>79</v>
@@ -7985,7 +7988,7 @@
         <v>79</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>77</v>
@@ -8003,24 +8006,24 @@
         <v>79</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AM54" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AN54" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AO54" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -8046,10 +8049,10 @@
         <v>91</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -8061,7 +8064,7 @@
         <v>79</v>
       </c>
       <c r="S55" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="T55" t="s" s="2">
         <v>79</v>
@@ -8100,7 +8103,7 @@
         <v>79</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>77</v>
@@ -8109,7 +8112,7 @@
         <v>89</v>
       </c>
       <c r="AI55" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AJ55" t="s" s="2">
         <v>79</v>
@@ -8124,7 +8127,7 @@
         <v>79</v>
       </c>
       <c r="AN55" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AO55" t="s" s="2">
         <v>79</v>
@@ -8132,14 +8135,14 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" t="s" s="2">
@@ -8161,13 +8164,13 @@
         <v>136</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="O56" s="2"/>
       <c r="P56" t="s" s="2">
@@ -8208,7 +8211,7 @@
         <v>139</v>
       </c>
       <c r="AC56" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AD56" t="s" s="2">
         <v>79</v>
@@ -8217,7 +8220,7 @@
         <v>140</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>77</v>
@@ -8241,7 +8244,7 @@
         <v>79</v>
       </c>
       <c r="AN56" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AO56" t="s" s="2">
         <v>79</v>
@@ -8249,10 +8252,10 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8275,16 +8278,16 @@
         <v>90</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="O57" s="2"/>
       <c r="P57" t="s" s="2">
@@ -8334,7 +8337,7 @@
         <v>79</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>77</v>
@@ -8358,7 +8361,7 @@
         <v>79</v>
       </c>
       <c r="AN57" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AO57" t="s" s="2">
         <v>134</v>
@@ -8366,10 +8369,10 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8392,13 +8395,13 @@
         <v>90</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
@@ -8449,7 +8452,7 @@
         <v>79</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>77</v>
@@ -8473,7 +8476,7 @@
         <v>79</v>
       </c>
       <c r="AN58" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AO58" t="s" s="2">
         <v>134</v>
@@ -8481,10 +8484,10 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8507,13 +8510,13 @@
         <v>90</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -8564,7 +8567,7 @@
         <v>79</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>89</v>
@@ -8588,7 +8591,7 @@
         <v>79</v>
       </c>
       <c r="AN59" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AO59" t="s" s="2">
         <v>134</v>

</xml_diff>

<commit_message>
update fichier svg 38064b15b5c158dc3025fb8fd49f742f0a182002
</commit_message>
<xml_diff>
--- a/update-mapping-pn13/ig/StructureDefinition-oncofair-careplan.xlsx
+++ b/update-mapping-pn13/ig/StructureDefinition-oncofair-careplan.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-27T09:43:00+00:00</t>
+    <t>2024-05-27T14:54:53+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -78,7 +78,8 @@
     <t>Description</t>
   </si>
   <si>
-    <t>This object describes the chaining of prescription elements attached to the prescribed protocol. Its structure enables the chaining of nested sub-protocols.</t>
+    <t>This object describes the chaining of prescription elements attached to the prescribed protocol. Its structure enables the chaining of nested sub-protocols. 
+Cet objet décrit le chaînage des éléments de prescription rattachés au protocole prescrit. Sa structure permet le chaînage de sous-protocoles imbriqués.</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -273,7 +274,7 @@
 dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().ofType(canonical) | %resource.descendants().ofType(uri) | %resource.descendants().ofType(url))) or descendants().where(reference = '#').exists() or descendants().where(ofType(canonical) = '#').exists() or descendants().where(ofType(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}</t>
   </si>
   <si>
-    <t>PROTOCOLE PRESCRIT</t>
+    <t>ProtocolePrescrit</t>
   </si>
   <si>
     <t>Request</t>

</xml_diff>

<commit_message>
Ajout des Title et de la requête SQL 633303c7e40dbcda13ce94479abd019e40f49819
</commit_message>
<xml_diff>
--- a/update-mapping-pn13/ig/StructureDefinition-oncofair-careplan.xlsx
+++ b/update-mapping-pn13/ig/StructureDefinition-oncofair-careplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2517" uniqueCount="474">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-17T15:49:27+00:00</t>
+    <t>2024-06-19T11:28:46+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -475,6 +475,9 @@
 </t>
   </si>
   <si>
+    <t>OncoFAIRCPTreatment</t>
+  </si>
+  <si>
     <t>Extension created as part of OncoFAIR grouping together the treatment number, the day number and the reference date and time of the prescribed protocol. 
 Extension créée dans le cadre d'OncoFAIR regroupant le numéro de cure, le numéro de jour ainsi que la date et heure de référence du protocole prescrit.</t>
   </si>
@@ -487,6 +490,9 @@
   <si>
     <t xml:space="preserve">Extension {http://ltsi.univ-rennes.fr/StructureDefinition/oncofair-pharmacist-advice}
 </t>
+  </si>
+  <si>
+    <t>OncoFAIRPharmacistAdvice</t>
   </si>
   <si>
     <t>Extension created as part of OncoFAIR containing the validation and pharmaceutical proposal. 
@@ -2940,10 +2946,10 @@
         <v>145</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -3026,13 +3032,13 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B11" t="s" s="2">
         <v>135</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D11" t="s" s="2">
         <v>79</v>
@@ -3054,13 +3060,13 @@
         <v>79</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="M11" t="s" s="2">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -3143,14 +3149,14 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" t="s" s="2">
@@ -3172,16 +3178,16 @@
         <v>136</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="N12" t="s" s="2">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="O12" t="s" s="2">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="P12" t="s" s="2">
         <v>79</v>
@@ -3230,7 +3236,7 @@
         <v>79</v>
       </c>
       <c r="AF12" t="s" s="2">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="AG12" t="s" s="2">
         <v>77</v>
@@ -3262,10 +3268,10 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
@@ -3288,19 +3294,19 @@
         <v>90</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="N13" t="s" s="2">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="O13" t="s" s="2">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="P13" t="s" s="2">
         <v>79</v>
@@ -3349,7 +3355,7 @@
         <v>79</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>77</v>
@@ -3364,27 +3370,27 @@
         <v>101</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="AN13" t="s" s="2">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="AO13" t="s" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -3410,10 +3416,10 @@
         <v>91</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
@@ -3464,7 +3470,7 @@
         <v>79</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>77</v>
@@ -3473,7 +3479,7 @@
         <v>89</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AJ14" t="s" s="2">
         <v>79</v>
@@ -3488,7 +3494,7 @@
         <v>79</v>
       </c>
       <c r="AN14" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AO14" t="s" s="2">
         <v>79</v>
@@ -3496,14 +3502,14 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" t="s" s="2">
@@ -3525,13 +3531,13 @@
         <v>136</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="O15" s="2"/>
       <c r="P15" t="s" s="2">
@@ -3572,7 +3578,7 @@
         <v>139</v>
       </c>
       <c r="AC15" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AD15" t="s" s="2">
         <v>79</v>
@@ -3581,7 +3587,7 @@
         <v>140</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>77</v>
@@ -3605,7 +3611,7 @@
         <v>79</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>79</v>
@@ -3613,10 +3619,10 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
@@ -3642,16 +3648,16 @@
         <v>109</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="O16" t="s" s="2">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="P16" t="s" s="2">
         <v>79</v>
@@ -3679,10 +3685,10 @@
         <v>113</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Z16" t="s" s="2">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="AA16" t="s" s="2">
         <v>79</v>
@@ -3700,7 +3706,7 @@
         <v>79</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>77</v>
@@ -3724,7 +3730,7 @@
         <v>79</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AO16" t="s" s="2">
         <v>134</v>
@@ -3732,10 +3738,10 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -3758,19 +3764,19 @@
         <v>90</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="O17" t="s" s="2">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="P17" t="s" s="2">
         <v>79</v>
@@ -3795,13 +3801,13 @@
         <v>79</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="Y17" t="s" s="2">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="Z17" t="s" s="2">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="AA17" t="s" s="2">
         <v>79</v>
@@ -3819,7 +3825,7 @@
         <v>79</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>77</v>
@@ -3843,18 +3849,18 @@
         <v>79</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="AO17" t="s" s="2">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3880,16 +3886,16 @@
         <v>103</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="O18" t="s" s="2">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="P18" t="s" s="2">
         <v>79</v>
@@ -3902,7 +3908,7 @@
         <v>79</v>
       </c>
       <c r="T18" t="s" s="2">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="U18" t="s" s="2">
         <v>79</v>
@@ -3938,7 +3944,7 @@
         <v>79</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>77</v>
@@ -3962,18 +3968,18 @@
         <v>79</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="AO18" t="s" s="2">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3996,16 +4002,16 @@
         <v>90</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" t="s" s="2">
@@ -4019,7 +4025,7 @@
         <v>79</v>
       </c>
       <c r="T19" t="s" s="2">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="U19" t="s" s="2">
         <v>79</v>
@@ -4055,7 +4061,7 @@
         <v>79</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>77</v>
@@ -4064,7 +4070,7 @@
         <v>89</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="AJ19" t="s" s="2">
         <v>101</v>
@@ -4079,18 +4085,18 @@
         <v>79</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="AO19" t="s" s="2">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -4113,13 +4119,13 @@
         <v>90</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
@@ -4170,7 +4176,7 @@
         <v>79</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>77</v>
@@ -4194,18 +4200,18 @@
         <v>79</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="AO20" t="s" s="2">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -4228,16 +4234,16 @@
         <v>90</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" t="s" s="2">
@@ -4287,7 +4293,7 @@
         <v>79</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>77</v>
@@ -4311,18 +4317,18 @@
         <v>79</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="AO21" t="s" s="2">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4345,13 +4351,13 @@
         <v>90</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
@@ -4402,7 +4408,7 @@
         <v>79</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>77</v>
@@ -4420,13 +4426,13 @@
         <v>79</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="AM22" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>79</v>
@@ -4434,10 +4440,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4463,13 +4469,13 @@
         <v>103</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="N23" t="s" s="2">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" t="s" s="2">
@@ -4519,7 +4525,7 @@
         <v>79</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>77</v>
@@ -4537,13 +4543,13 @@
         <v>79</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="AM23" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>79</v>
@@ -4551,14 +4557,14 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s" s="2">
@@ -4577,17 +4583,17 @@
         <v>90</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="P24" t="s" s="2">
         <v>79</v>
@@ -4636,7 +4642,7 @@
         <v>79</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>77</v>
@@ -4654,7 +4660,7 @@
         <v>84</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AM24" t="s" s="2">
         <v>79</v>
@@ -4668,14 +4674,14 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" t="s" s="2">
@@ -4694,19 +4700,19 @@
         <v>90</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="O25" t="s" s="2">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="P25" t="s" s="2">
         <v>79</v>
@@ -4755,7 +4761,7 @@
         <v>79</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>77</v>
@@ -4773,7 +4779,7 @@
         <v>79</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="AM25" t="s" s="2">
         <v>79</v>
@@ -4787,10 +4793,10 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4813,16 +4819,16 @@
         <v>90</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" t="s" s="2">
@@ -4872,7 +4878,7 @@
         <v>79</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>77</v>
@@ -4904,10 +4910,10 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4933,16 +4939,16 @@
         <v>109</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="O27" t="s" s="2">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="P27" t="s" s="2">
         <v>79</v>
@@ -4970,28 +4976,28 @@
         <v>113</v>
       </c>
       <c r="Y27" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="Z27" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="AA27" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AB27" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AC27" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AD27" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AE27" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AF27" t="s" s="2">
         <v>266</v>
-      </c>
-      <c r="Z27" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="AA27" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AB27" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AC27" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AD27" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AE27" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AF27" t="s" s="2">
-        <v>264</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>89</v>
@@ -5006,27 +5012,27 @@
         <v>101</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -5052,16 +5058,16 @@
         <v>109</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="O28" t="s" s="2">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="P28" t="s" s="2">
         <v>79</v>
@@ -5089,10 +5095,10 @@
         <v>113</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="Z28" t="s" s="2">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="AA28" t="s" s="2">
         <v>79</v>
@@ -5110,7 +5116,7 @@
         <v>79</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>89</v>
@@ -5128,7 +5134,7 @@
         <v>79</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="AM28" t="s" s="2">
         <v>79</v>
@@ -5142,10 +5148,10 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -5168,19 +5174,19 @@
         <v>90</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="O29" t="s" s="2">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="P29" t="s" s="2">
         <v>79</v>
@@ -5205,13 +5211,13 @@
         <v>79</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="Z29" t="s" s="2">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="AA29" t="s" s="2">
         <v>79</v>
@@ -5229,7 +5235,7 @@
         <v>79</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>77</v>
@@ -5250,7 +5256,7 @@
         <v>79</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>79</v>
@@ -5261,10 +5267,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5287,13 +5293,13 @@
         <v>90</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -5344,7 +5350,7 @@
         <v>79</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>77</v>
@@ -5359,7 +5365,7 @@
         <v>101</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>79</v>
@@ -5376,10 +5382,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5402,17 +5408,17 @@
         <v>90</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>79</v>
@@ -5461,7 +5467,7 @@
         <v>79</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>77</v>
@@ -5482,7 +5488,7 @@
         <v>79</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>79</v>
@@ -5493,14 +5499,14 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" t="s" s="2">
@@ -5519,13 +5525,13 @@
         <v>90</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -5576,7 +5582,7 @@
         <v>79</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>89</v>
@@ -5594,24 +5600,24 @@
         <v>79</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="AO32" t="s" s="2">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5634,16 +5640,16 @@
         <v>90</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="N33" t="s" s="2">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" t="s" s="2">
@@ -5693,7 +5699,7 @@
         <v>79</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>77</v>
@@ -5711,28 +5717,28 @@
         <v>79</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="AO33" t="s" s="2">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" t="s" s="2">
@@ -5751,19 +5757,19 @@
         <v>90</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="N34" t="s" s="2">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="O34" t="s" s="2">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="P34" t="s" s="2">
         <v>79</v>
@@ -5812,7 +5818,7 @@
         <v>79</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>77</v>
@@ -5830,28 +5836,28 @@
         <v>79</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="AO34" t="s" s="2">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" t="s" s="2">
@@ -5870,13 +5876,13 @@
         <v>90</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -5927,7 +5933,7 @@
         <v>79</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>77</v>
@@ -5945,13 +5951,13 @@
         <v>79</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="AO35" t="s" s="2">
         <v>79</v>
@@ -5959,10 +5965,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5985,16 +5991,16 @@
         <v>90</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="N36" t="s" s="2">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="O36" s="2"/>
       <c r="P36" t="s" s="2">
@@ -6044,7 +6050,7 @@
         <v>79</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>77</v>
@@ -6062,10 +6068,10 @@
         <v>79</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>79</v>
@@ -6076,10 +6082,10 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6102,16 +6108,16 @@
         <v>79</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="N37" t="s" s="2">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="O37" s="2"/>
       <c r="P37" t="s" s="2">
@@ -6161,7 +6167,7 @@
         <v>79</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>77</v>
@@ -6193,10 +6199,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6219,17 +6225,17 @@
         <v>79</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>79</v>
@@ -6278,7 +6284,7 @@
         <v>79</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>77</v>
@@ -6296,10 +6302,10 @@
         <v>79</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>79</v>
@@ -6310,10 +6316,10 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6336,19 +6342,19 @@
         <v>90</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="O39" t="s" s="2">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="P39" t="s" s="2">
         <v>79</v>
@@ -6373,13 +6379,13 @@
         <v>79</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="Z39" t="s" s="2">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="AA39" t="s" s="2">
         <v>79</v>
@@ -6397,7 +6403,7 @@
         <v>79</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>77</v>
@@ -6415,24 +6421,24 @@
         <v>79</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="AN39" t="s" s="2">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="AO39" t="s" s="2">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6455,19 +6461,19 @@
         <v>79</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="O40" t="s" s="2">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="P40" t="s" s="2">
         <v>79</v>
@@ -6516,7 +6522,7 @@
         <v>79</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>77</v>
@@ -6534,7 +6540,7 @@
         <v>79</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>79</v>
@@ -6548,10 +6554,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6574,19 +6580,19 @@
         <v>79</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="O41" t="s" s="2">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="P41" t="s" s="2">
         <v>79</v>
@@ -6635,7 +6641,7 @@
         <v>79</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>77</v>
@@ -6659,18 +6665,18 @@
         <v>79</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="AO41" t="s" s="2">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6693,17 +6699,17 @@
         <v>79</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="P42" t="s" s="2">
         <v>79</v>
@@ -6752,7 +6758,7 @@
         <v>79</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>77</v>
@@ -6770,13 +6776,13 @@
         <v>79</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="AM42" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="AO42" t="s" s="2">
         <v>79</v>
@@ -6784,10 +6790,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6810,13 +6816,13 @@
         <v>79</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -6867,7 +6873,7 @@
         <v>79</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>77</v>
@@ -6876,7 +6882,7 @@
         <v>89</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>79</v>
@@ -6891,7 +6897,7 @@
         <v>79</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AO43" t="s" s="2">
         <v>79</v>
@@ -6899,14 +6905,14 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" t="s" s="2">
@@ -6928,13 +6934,13 @@
         <v>136</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="O44" s="2"/>
       <c r="P44" t="s" s="2">
@@ -6984,7 +6990,7 @@
         <v>79</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>77</v>
@@ -7008,7 +7014,7 @@
         <v>79</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AO44" t="s" s="2">
         <v>79</v>
@@ -7016,14 +7022,14 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s" s="2">
@@ -7045,16 +7051,16 @@
         <v>136</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="O45" t="s" s="2">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="P45" t="s" s="2">
         <v>79</v>
@@ -7103,7 +7109,7 @@
         <v>79</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>77</v>
@@ -7135,10 +7141,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -7161,19 +7167,19 @@
         <v>79</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="O46" t="s" s="2">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="P46" t="s" s="2">
         <v>79</v>
@@ -7198,13 +7204,13 @@
         <v>79</v>
       </c>
       <c r="X46" t="s" s="2">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="Y46" t="s" s="2">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="Z46" t="s" s="2">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="AA46" t="s" s="2">
         <v>79</v>
@@ -7222,7 +7228,7 @@
         <v>79</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>77</v>
@@ -7240,13 +7246,13 @@
         <v>79</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="AM46" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AN46" t="s" s="2">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="AO46" t="s" s="2">
         <v>79</v>
@@ -7254,10 +7260,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7280,19 +7286,19 @@
         <v>79</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="O47" t="s" s="2">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="P47" t="s" s="2">
         <v>79</v>
@@ -7341,7 +7347,7 @@
         <v>79</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>77</v>
@@ -7365,18 +7371,18 @@
         <v>79</v>
       </c>
       <c r="AN47" t="s" s="2">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="AO47" t="s" s="2">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7399,19 +7405,19 @@
         <v>79</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="O48" t="s" s="2">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="P48" t="s" s="2">
         <v>79</v>
@@ -7460,7 +7466,7 @@
         <v>79</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>77</v>
@@ -7478,13 +7484,13 @@
         <v>79</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="AM48" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="AO48" t="s" s="2">
         <v>79</v>
@@ -7492,10 +7498,10 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7518,17 +7524,17 @@
         <v>79</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="P49" t="s" s="2">
         <v>79</v>
@@ -7565,7 +7571,7 @@
         <v>79</v>
       </c>
       <c r="AB49" t="s" s="2">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="AC49" s="2"/>
       <c r="AD49" t="s" s="2">
@@ -7575,7 +7581,7 @@
         <v>140</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>77</v>
@@ -7593,27 +7599,27 @@
         <v>79</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="AM49" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="AO49" t="s" s="2">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C50" t="s" s="2">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="D50" t="s" s="2">
         <v>79</v>
@@ -7635,17 +7641,17 @@
         <v>79</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="P50" t="s" s="2">
         <v>79</v>
@@ -7694,7 +7700,7 @@
         <v>79</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>77</v>
@@ -7709,27 +7715,27 @@
         <v>101</v>
       </c>
       <c r="AK50" t="s" s="2">
+        <v>430</v>
+      </c>
+      <c r="AL50" t="s" s="2">
         <v>428</v>
       </c>
-      <c r="AL50" t="s" s="2">
-        <v>426</v>
-      </c>
       <c r="AM50" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7755,10 +7761,10 @@
         <v>91</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -7770,7 +7776,7 @@
         <v>79</v>
       </c>
       <c r="S51" t="s" s="2">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="T51" t="s" s="2">
         <v>79</v>
@@ -7809,7 +7815,7 @@
         <v>79</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>77</v>
@@ -7818,7 +7824,7 @@
         <v>89</v>
       </c>
       <c r="AI51" t="s" s="2">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AJ51" t="s" s="2">
         <v>79</v>
@@ -7833,7 +7839,7 @@
         <v>79</v>
       </c>
       <c r="AN51" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AO51" t="s" s="2">
         <v>79</v>
@@ -7841,14 +7847,14 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" t="s" s="2">
@@ -7870,13 +7876,13 @@
         <v>136</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="O52" s="2"/>
       <c r="P52" t="s" s="2">
@@ -7917,7 +7923,7 @@
         <v>139</v>
       </c>
       <c r="AC52" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AD52" t="s" s="2">
         <v>79</v>
@@ -7926,7 +7932,7 @@
         <v>140</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>77</v>
@@ -7950,7 +7956,7 @@
         <v>79</v>
       </c>
       <c r="AN52" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AO52" t="s" s="2">
         <v>79</v>
@@ -7958,10 +7964,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7984,16 +7990,16 @@
         <v>90</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="O53" s="2"/>
       <c r="P53" t="s" s="2">
@@ -8043,7 +8049,7 @@
         <v>79</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>77</v>
@@ -8067,7 +8073,7 @@
         <v>79</v>
       </c>
       <c r="AN53" t="s" s="2">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="AO53" t="s" s="2">
         <v>134</v>
@@ -8075,10 +8081,10 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -8101,13 +8107,13 @@
         <v>90</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
@@ -8158,7 +8164,7 @@
         <v>79</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>77</v>
@@ -8182,7 +8188,7 @@
         <v>79</v>
       </c>
       <c r="AN54" t="s" s="2">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="AO54" t="s" s="2">
         <v>134</v>
@@ -8190,10 +8196,10 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -8216,13 +8222,13 @@
         <v>90</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -8273,7 +8279,7 @@
         <v>79</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>89</v>
@@ -8297,7 +8303,7 @@
         <v>79</v>
       </c>
       <c r="AN55" t="s" s="2">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="AO55" t="s" s="2">
         <v>134</v>
@@ -8305,13 +8311,13 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C56" t="s" s="2">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="D56" t="s" s="2">
         <v>79</v>
@@ -8333,17 +8339,17 @@
         <v>79</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="P56" t="s" s="2">
         <v>79</v>
@@ -8392,7 +8398,7 @@
         <v>79</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>77</v>
@@ -8407,27 +8413,27 @@
         <v>101</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="AM56" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AN56" t="s" s="2">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="AO56" t="s" s="2">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8453,10 +8459,10 @@
         <v>91</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
@@ -8468,7 +8474,7 @@
         <v>79</v>
       </c>
       <c r="S57" t="s" s="2">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="T57" t="s" s="2">
         <v>79</v>
@@ -8507,7 +8513,7 @@
         <v>79</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>77</v>
@@ -8516,7 +8522,7 @@
         <v>89</v>
       </c>
       <c r="AI57" t="s" s="2">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AJ57" t="s" s="2">
         <v>79</v>
@@ -8531,7 +8537,7 @@
         <v>79</v>
       </c>
       <c r="AN57" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AO57" t="s" s="2">
         <v>79</v>
@@ -8539,14 +8545,14 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" t="s" s="2">
@@ -8568,13 +8574,13 @@
         <v>136</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="O58" s="2"/>
       <c r="P58" t="s" s="2">
@@ -8615,7 +8621,7 @@
         <v>139</v>
       </c>
       <c r="AC58" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AD58" t="s" s="2">
         <v>79</v>
@@ -8624,7 +8630,7 @@
         <v>140</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>77</v>
@@ -8648,7 +8654,7 @@
         <v>79</v>
       </c>
       <c r="AN58" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AO58" t="s" s="2">
         <v>79</v>
@@ -8656,10 +8662,10 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8682,16 +8688,16 @@
         <v>90</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="O59" s="2"/>
       <c r="P59" t="s" s="2">
@@ -8741,7 +8747,7 @@
         <v>79</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>77</v>
@@ -8765,7 +8771,7 @@
         <v>79</v>
       </c>
       <c r="AN59" t="s" s="2">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="AO59" t="s" s="2">
         <v>134</v>
@@ -8773,10 +8779,10 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8799,13 +8805,13 @@
         <v>90</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="N60" s="2"/>
       <c r="O60" s="2"/>
@@ -8856,7 +8862,7 @@
         <v>79</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>77</v>
@@ -8880,7 +8886,7 @@
         <v>79</v>
       </c>
       <c r="AN60" t="s" s="2">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="AO60" t="s" s="2">
         <v>134</v>
@@ -8888,10 +8894,10 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -8914,13 +8920,13 @@
         <v>90</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -8971,7 +8977,7 @@
         <v>79</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>89</v>
@@ -8995,7 +9001,7 @@
         <v>79</v>
       </c>
       <c r="AN61" t="s" s="2">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="AO61" t="s" s="2">
         <v>134</v>
@@ -9003,13 +9009,13 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="C62" t="s" s="2">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="D62" t="s" s="2">
         <v>79</v>
@@ -9031,17 +9037,17 @@
         <v>79</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="P62" t="s" s="2">
         <v>79</v>
@@ -9090,7 +9096,7 @@
         <v>79</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>77</v>
@@ -9108,24 +9114,24 @@
         <v>79</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="AM62" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AN62" t="s" s="2">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="AO62" t="s" s="2">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9151,10 +9157,10 @@
         <v>91</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -9166,7 +9172,7 @@
         <v>79</v>
       </c>
       <c r="S63" t="s" s="2">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="T63" t="s" s="2">
         <v>79</v>
@@ -9205,7 +9211,7 @@
         <v>79</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>77</v>
@@ -9214,7 +9220,7 @@
         <v>89</v>
       </c>
       <c r="AI63" t="s" s="2">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AJ63" t="s" s="2">
         <v>79</v>
@@ -9229,7 +9235,7 @@
         <v>79</v>
       </c>
       <c r="AN63" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AO63" t="s" s="2">
         <v>79</v>
@@ -9237,14 +9243,14 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" t="s" s="2">
@@ -9266,13 +9272,13 @@
         <v>136</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="N64" t="s" s="2">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="O64" s="2"/>
       <c r="P64" t="s" s="2">
@@ -9313,7 +9319,7 @@
         <v>139</v>
       </c>
       <c r="AC64" t="s" s="2">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AD64" t="s" s="2">
         <v>79</v>
@@ -9322,7 +9328,7 @@
         <v>140</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>77</v>
@@ -9346,7 +9352,7 @@
         <v>79</v>
       </c>
       <c r="AN64" t="s" s="2">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AO64" t="s" s="2">
         <v>79</v>
@@ -9354,10 +9360,10 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9380,16 +9386,16 @@
         <v>90</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="N65" t="s" s="2">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="O65" s="2"/>
       <c r="P65" t="s" s="2">
@@ -9439,7 +9445,7 @@
         <v>79</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="AG65" t="s" s="2">
         <v>77</v>
@@ -9463,7 +9469,7 @@
         <v>79</v>
       </c>
       <c r="AN65" t="s" s="2">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="AO65" t="s" s="2">
         <v>134</v>
@@ -9471,10 +9477,10 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -9497,13 +9503,13 @@
         <v>90</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
@@ -9554,7 +9560,7 @@
         <v>79</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>77</v>
@@ -9578,7 +9584,7 @@
         <v>79</v>
       </c>
       <c r="AN66" t="s" s="2">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="AO66" t="s" s="2">
         <v>134</v>
@@ -9586,10 +9592,10 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
@@ -9612,13 +9618,13 @@
         <v>90</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="N67" s="2"/>
       <c r="O67" s="2"/>
@@ -9669,7 +9675,7 @@
         <v>79</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>89</v>
@@ -9693,7 +9699,7 @@
         <v>79</v>
       </c>
       <c r="AN67" t="s" s="2">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="AO67" t="s" s="2">
         <v>134</v>

</xml_diff>